<commit_message>
D3_algorithm_MS readded by removing temporary files
</commit_message>
<xml_diff>
--- a/i_codebooks/D3_algorithms_MS.xlsx
+++ b/i_codebooks/D3_algorithms_MS.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20404"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rosgin2\Documents\DP3-MS-SLE\i_codebooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davide\Documents\Git repositories\Work\DP3-MS-SLE\i_codebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE5F71F-419E-4FC5-86FD-D5EFF40A615B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19416" windowHeight="8760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19410" windowHeight="8760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -63,9 +64,6 @@
   </si>
   <si>
     <t>Primary key</t>
-  </si>
-  <si>
-    <t>person_id algorithm</t>
   </si>
   <si>
     <t>Variable</t>
@@ -146,11 +144,14 @@
   <si>
     <t>value</t>
   </si>
+  <si>
+    <t>person_id algorithm</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
@@ -318,7 +319,7 @@
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -530,19 +531,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="32.6640625" customWidth="1"/>
-    <col min="2" max="2" width="144.6640625" customWidth="1"/>
-    <col min="3" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="32.7109375" customWidth="1"/>
+    <col min="2" max="2" width="144.7109375" customWidth="1"/>
+    <col min="3" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.4">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -550,7 +553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.6">
+    <row r="2" spans="1:2" ht="15.75">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -558,7 +561,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.6">
+    <row r="3" spans="1:2" ht="15.75">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -566,7 +569,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.6">
+    <row r="4" spans="1:2" ht="15.75">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -574,7 +577,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.6">
+    <row r="5" spans="1:2" ht="15.75">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -582,57 +585,57 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.6">
+    <row r="6" spans="1:2" ht="15.75">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="5"/>
     </row>
-    <row r="7" spans="1:2" ht="15.6">
+    <row r="7" spans="1:2" ht="15.75">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="14.4">
+    <row r="8" spans="1:2">
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:2" ht="14.4">
+    <row r="9" spans="1:2">
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:2" ht="14.4">
+    <row r="10" spans="1:2">
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:2" ht="14.4">
+    <row r="11" spans="1:2">
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:2" ht="14.4">
+    <row r="12" spans="1:2">
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:2" ht="14.4">
+    <row r="13" spans="1:2">
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:2" ht="14.4">
+    <row r="14" spans="1:2">
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:2" ht="14.4">
+    <row r="15" spans="1:2">
       <c r="B15" s="2"/>
     </row>
-    <row r="16" spans="1:2" ht="14.4">
+    <row r="16" spans="1:2">
       <c r="B16" s="2"/>
     </row>
-    <row r="17" spans="2:2" ht="14.4">
+    <row r="17" spans="2:2">
       <c r="B17" s="2"/>
     </row>
-    <row r="18" spans="2:2" ht="14.4">
+    <row r="18" spans="2:2">
       <c r="B18" s="2"/>
     </row>
-    <row r="19" spans="2:2" ht="14.4">
+    <row r="19" spans="2:2">
       <c r="B19" s="2"/>
     </row>
-    <row r="20" spans="2:2" ht="14.4">
+    <row r="20" spans="2:2">
       <c r="B20" s="2"/>
     </row>
     <row r="21" spans="2:2" ht="15.75" customHeight="1">
@@ -3582,7 +3585,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z899"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3592,39 +3595,39 @@
       <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="60.109375" customWidth="1"/>
+    <col min="1" max="1" width="60.140625" customWidth="1"/>
     <col min="2" max="2" width="64" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="99.6640625" customWidth="1"/>
-    <col min="5" max="5" width="25.6640625" customWidth="1"/>
-    <col min="6" max="6" width="34.109375" customWidth="1"/>
-    <col min="7" max="7" width="25.6640625" customWidth="1"/>
-    <col min="8" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="99.7109375" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" customWidth="1"/>
+    <col min="6" max="6" width="34.140625" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" customWidth="1"/>
+    <col min="8" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="14.4">
+    <row r="1" spans="1:26">
       <c r="A1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="11" t="s">
         <v>18</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>19</v>
       </c>
       <c r="H1" s="12"/>
       <c r="I1" s="12"/>
@@ -3648,16 +3651,16 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
       <c r="A2" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="C2" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="D2" s="13" t="s">
         <v>22</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>23</v>
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="2"/>
@@ -3682,15 +3685,15 @@
       <c r="Y2" s="12"/>
       <c r="Z2" s="12"/>
     </row>
-    <row r="3" spans="1:26" ht="14.4">
+    <row r="3" spans="1:26">
       <c r="A3" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="14" t="s">
-        <v>25</v>
-      </c>
       <c r="C3" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="2"/>
@@ -3716,24 +3719,24 @@
       <c r="Y3" s="12"/>
       <c r="Z3" s="12"/>
     </row>
-    <row r="4" spans="1:26" ht="72">
+    <row r="4" spans="1:26" ht="75">
       <c r="A4" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="C4" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="D4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="E4" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="F4" s="17" t="s">
         <v>30</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>31</v>
       </c>
       <c r="G4" s="16"/>
       <c r="H4" s="12"/>
@@ -28823,97 +28826,97 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C997"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="28.44140625" customWidth="1"/>
-    <col min="2" max="2" width="83.5546875" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" customWidth="1"/>
+    <col min="2" max="2" width="83.5703125" customWidth="1"/>
     <col min="3" max="3" width="68" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14.4">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:3" ht="14.4">
+    <row r="2" spans="1:3">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3" ht="14.4">
+    <row r="3" spans="1:3">
       <c r="A3" s="12"/>
       <c r="B3" s="12"/>
       <c r="C3" s="2"/>
     </row>
-    <row r="4" spans="1:3" ht="14.4">
+    <row r="4" spans="1:3">
       <c r="A4" s="12"/>
       <c r="B4" s="12"/>
       <c r="C4" s="2"/>
     </row>
-    <row r="5" spans="1:3" ht="14.4">
+    <row r="5" spans="1:3">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
       <c r="C5" s="2"/>
     </row>
-    <row r="6" spans="1:3" ht="14.4">
+    <row r="6" spans="1:3">
       <c r="A6" s="12"/>
       <c r="B6" s="12"/>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:3" ht="14.4">
+    <row r="7" spans="1:3">
       <c r="A7" s="12"/>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:3" ht="14.4">
+    <row r="8" spans="1:3">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:3" ht="14.4">
+    <row r="9" spans="1:3">
       <c r="A9" s="12"/>
       <c r="B9" s="12"/>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:3" ht="14.4">
+    <row r="10" spans="1:3">
       <c r="A10" s="12"/>
       <c r="B10" s="12"/>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:3" ht="14.4">
+    <row r="11" spans="1:3">
       <c r="A11" s="12"/>
       <c r="B11" s="12"/>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:3" ht="14.4">
+    <row r="12" spans="1:3">
       <c r="A12" s="12"/>
       <c r="B12" s="12"/>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:3" ht="14.4">
+    <row r="13" spans="1:3">
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:3" ht="14.4">
+    <row r="14" spans="1:3">
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:3" ht="14.4">
+    <row r="15" spans="1:3">
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="1:3" ht="14.4">
+    <row r="16" spans="1:3">
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="3:3" ht="14.4">
+    <row r="17" spans="3:3">
       <c r="C17" s="2"/>
     </row>
     <row r="18" spans="3:3" ht="15.75" customHeight="1">
@@ -31863,81 +31866,81 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I990"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" customWidth="1"/>
-    <col min="5" max="5" width="19.44140625" customWidth="1"/>
-    <col min="6" max="6" width="21.109375" customWidth="1"/>
-    <col min="7" max="7" width="10.88671875" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" customWidth="1"/>
-    <col min="9" max="9" width="18.44140625" customWidth="1"/>
-    <col min="10" max="10" width="19.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" customWidth="1"/>
     <col min="11" max="11" width="38" customWidth="1"/>
-    <col min="12" max="12" width="61.109375" customWidth="1"/>
-    <col min="13" max="26" width="8.6640625" customWidth="1"/>
+    <col min="12" max="12" width="61.140625" customWidth="1"/>
+    <col min="13" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14.4">
+    <row r="1" spans="1:9">
       <c r="A1" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D1" s="13"/>
       <c r="E1" s="18"/>
       <c r="F1" s="13"/>
     </row>
-    <row r="2" spans="1:9" ht="14.4">
+    <row r="2" spans="1:9">
       <c r="A2" s="19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" s="20">
         <v>40551</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" ht="14.4">
+    <row r="3" spans="1:9">
       <c r="A3" s="19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" s="20">
         <v>40559</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" ht="14.4">
+    <row r="4" spans="1:9">
       <c r="A4" s="17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" s="21">
         <v>42452</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.75" customHeight="1"/>

</xml_diff>